<commit_message>
Final Excel MM changes
</commit_message>
<xml_diff>
--- a/Money Matters/Money Matters.xlsx
+++ b/Money Matters/Money Matters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliangriffin/Desktop/RBC/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliangriffin/Desktop/NewExcel_Projects_Local/NewExcel_Projects/Money Matters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F886CE9-1AC4-2649-B5D0-F7BFCAE99494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D010B88-72A0-9D46-B49A-873640319078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId13"/>
+    <pivotCache cacheId="1" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3120" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3122" uniqueCount="115">
   <si>
     <t>Method</t>
   </si>
@@ -730,6 +730,12 @@
   <si>
     <t>Money Matters: Dashboard</t>
   </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t>The sheet is protected so only the slicers and chart fields are avalable for change.</t>
+  </si>
 </sst>
 </file>
 
@@ -1219,7 +1225,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -1289,6 +1295,20 @@
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="3" builtinId="37"/>
@@ -1296,7 +1316,37 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{0CBFBBA0-2B04-F540-AA3A-5B59D7AB2613}"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="42">
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4434,7 +4484,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-1AB5-2A46-B1F2-56118BFEC33A}"/>
+              <c16:uniqueId val="{00000001-21FF-3C48-9C68-58BEE80C1D24}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8320,8 +8370,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>226464</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="8" name="Category">
@@ -8344,7 +8394,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8383,7 +8433,7 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
-    <xdr:clientData/>
+    <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
@@ -8398,8 +8448,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>148251</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:tsle="http://schemas.microsoft.com/office/drawing/2012/timeslicer">
-      <mc:Choice Requires="tsle">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:tsle="http://schemas.microsoft.com/office/drawing/2012/timeslicer" Requires="tsle">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="9" name="Transaction Date">
@@ -8417,12 +8467,12 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2012/timeslicer">
-              <tsle:timeslicer name="Transaction Date"/>
+              <tsle:timeslicer xmlns:tsle="http://schemas.microsoft.com/office/drawing/2012/timeslicer" name="Transaction Date"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8460,7 +8510,7 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
-    <xdr:clientData/>
+    <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
@@ -8475,8 +8525,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>239037</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="10" name="Workday/Extended Weekend (inc Friday)">
@@ -8499,7 +8549,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8538,7 +8588,7 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
-    <xdr:clientData/>
+    <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
@@ -8553,8 +8603,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>173398</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="11" name="Method">
@@ -8577,7 +8627,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8616,7 +8666,7 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
-    <xdr:clientData/>
+    <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
@@ -8705,13 +8755,13 @@
       <xdr:rowOff>12702</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>897467</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5944</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Month">
@@ -8734,7 +8784,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8744,7 +8794,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2956886" y="2720914"/>
+              <a:off x="2948475" y="2720914"/>
               <a:ext cx="1944025" cy="1384634"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -8773,7 +8823,7 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
-    <xdr:clientData/>
+    <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
@@ -11832,7 +11882,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EB3F11B9-D113-7F4A-91F0-B3EFC801EA5E}" name="pivot_category" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EB3F11B9-D113-7F4A-91F0-B3EFC801EA5E}" name="pivot_category" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField showAll="0">
@@ -12039,7 +12089,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{971C53EE-E45E-FF4C-955C-416D24A2441E}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{971C53EE-E45E-FF4C-955C-416D24A2441E}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B45" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0">
@@ -12379,7 +12429,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4EE3A639-4420-FA42-BED3-A9AF713D5EBD}" name="expenses_table" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12" rowHeaderCaption="Category" colHeaderCaption="DOW">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4EE3A639-4420-FA42-BED3-A9AF713D5EBD}" name="expenses_table" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12" rowHeaderCaption="Category" colHeaderCaption="DOW">
   <location ref="A5:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisPage" showAll="0">
@@ -12585,7 +12635,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7DA7F608-522A-7B4A-A0D7-DCA332F361E7}" name="earnings_pivot" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="25" rowHeaderCaption="Category" colHeaderCaption="Month">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7DA7F608-522A-7B4A-A0D7-DCA332F361E7}" name="earnings_pivot" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="25" rowHeaderCaption="Category" colHeaderCaption="Month">
   <location ref="A4:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField showAll="0">
@@ -12845,7 +12895,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{673BB614-F46B-1243-97E1-B14448CFB4EC}" name="earnings_pivot" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19" rowHeaderCaption="Category" colHeaderCaption="Month">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{673BB614-F46B-1243-97E1-B14448CFB4EC}" name="earnings_pivot" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19" rowHeaderCaption="Category" colHeaderCaption="Month">
   <location ref="A4:E10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisPage" showAll="0">
@@ -12995,6 +13045,50 @@
   <dataFields count="1">
     <dataField name="Total Amount ($)" fld="4" baseField="0" baseItem="0" numFmtId="7"/>
   </dataFields>
+  <formats count="10">
+    <format dxfId="0">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="2">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="3">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="4">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="5">
+      <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="7" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="3">
+            <x v="16"/>
+            <x v="24"/>
+            <x v="46"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+  </formats>
   <chartFormats count="6">
     <chartFormat chart="10" format="10" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
@@ -13082,7 +13176,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D3F80AAA-42CD-A342-8A8D-09149152666B}" name="expenses_table" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11" rowHeaderCaption="Category" colHeaderCaption="DOW">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D3F80AAA-42CD-A342-8A8D-09149152666B}" name="expenses_table" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11" rowHeaderCaption="Category" colHeaderCaption="DOW">
   <location ref="A5:D18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisPage" showAll="0">
@@ -13197,7 +13291,7 @@
     <dataField name="Total Amount ($)" fld="4" baseField="0" baseItem="0" numFmtId="42"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="10">
+    <format dxfId="20">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -13399,7 +13493,7 @@
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
-  <slicer name="Category" xr10:uid="{0A837B24-03E4-BC49-A9E8-016206E296D2}" cache="Slicer_Category" caption="Category" startItem="5" style="SlicerStyleDark4" rowHeight="230716"/>
+  <slicer name="Category" xr10:uid="{0A837B24-03E4-BC49-A9E8-016206E296D2}" cache="Slicer_Category" caption="Category" startItem="2" style="SlicerStyleDark4" rowHeight="230716"/>
   <slicer name="Workday/Extended Weekend (inc Friday)" xr10:uid="{4B451EC3-F6B6-8144-8073-FE6A8C21501B}" cache="Slicer_Workday_Extended_Weekend__inc_Friday" caption="Workday/Extended Weekend (inc Friday)" style="SlicerStyleDark4" rowHeight="230716"/>
   <slicer name="Method" xr10:uid="{6F0F8EF4-E08B-D347-92F2-692DF2824AF1}" cache="Slicer_Method" caption="Payment Method" style="SlicerStyleDark4" rowHeight="230716"/>
 </slicers>
@@ -13418,7 +13512,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1CE2BBCA-3F43-EA48-9EC4-0007134C9FBC}" name="expenses_table" displayName="expenses_table" ref="A1:I247" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1CE2BBCA-3F43-EA48-9EC4-0007134C9FBC}" name="expenses_table" displayName="expenses_table" ref="A1:I247" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39">
   <autoFilter ref="A1:I247" xr:uid="{1CE2BBCA-3F43-EA48-9EC4-0007134C9FBC}">
     <filterColumn colId="4">
       <customFilters>
@@ -13431,18 +13525,18 @@
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F10CA1B2-7120-C84C-8023-87180B21085B}" name="Method"/>
-    <tableColumn id="2" xr3:uid="{1B439FAA-0761-C44E-965D-469A22852A8F}" name="Transaction Date" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{1B439FAA-0761-C44E-965D-469A22852A8F}" name="Transaction Date" dataDxfId="38"/>
     <tableColumn id="3" xr3:uid="{CC2B1945-8262-9145-9F19-C2DE98427053}" name="Category"/>
     <tableColumn id="4" xr3:uid="{A13631DC-44F7-D247-9F04-999BA9E49159}" name="Merchant"/>
     <tableColumn id="5" xr3:uid="{92221C3F-3723-3E46-9028-2994DF171F8A}" name="Amount ($)"/>
-    <tableColumn id="9" xr3:uid="{5E07B6B1-B6A7-FD45-A36B-AE02CF6A75AA}" name="Spending or Income" dataDxfId="27">
+    <tableColumn id="9" xr3:uid="{5E07B6B1-B6A7-FD45-A36B-AE02CF6A75AA}" name="Spending or Income" dataDxfId="37">
       <calculatedColumnFormula>IF(expenses_table[[#This Row],[Amount ($)]]&lt;0, "Spending", "Income")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{C747EDCA-AF62-A541-9179-3179FBEC7C11}" name="Need/Want"/>
-    <tableColumn id="7" xr3:uid="{38B9BC3B-CEB7-1246-A416-997FA882D8A9}" name="Month" dataDxfId="26">
+    <tableColumn id="7" xr3:uid="{38B9BC3B-CEB7-1246-A416-997FA882D8A9}" name="Month" dataDxfId="36">
       <calculatedColumnFormula>TEXT(expenses_table[[#This Row],[Transaction Date]], "mmmm")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{821F97FE-09B4-E647-907B-FEFE3B9E94F7}" name="Workday/Extended Weekend (inc Friday)" dataDxfId="25">
+    <tableColumn id="8" xr3:uid="{821F97FE-09B4-E647-907B-FEFE3B9E94F7}" name="Workday/Extended Weekend (inc Friday)" dataDxfId="35">
       <calculatedColumnFormula>IF(WEEKDAY(expenses_table[[#This Row],[Transaction Date]], 2) &lt;= 4, "Workday", "Ext-Weekend")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13451,7 +13545,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1B6A8F48-A898-7B41-8B2F-2C8E9106DD5A}" name="earnings_table" displayName="earnings_table" ref="A1:I247" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1B6A8F48-A898-7B41-8B2F-2C8E9106DD5A}" name="earnings_table" displayName="earnings_table" ref="A1:I247" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="A1:I247" xr:uid="{1B6A8F48-A898-7B41-8B2F-2C8E9106DD5A}">
     <filterColumn colId="2">
       <filters>
@@ -13467,22 +13561,22 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{31B2C3DA-4854-9844-9496-96146F16A89E}" name="Method" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{F71D2D76-F449-6846-A86A-31D132D01864}" name="Transaction Date" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{698BE150-94AA-6647-A4A5-F0D1632492E8}" name="Category" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{62EA866A-6213-BE46-A5CC-E8DAC9C406A8}" name="Merchant" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{28935B6D-449E-5A45-AA26-1E8220AE2B4F}" name="Amount ($)" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{FD1C89E1-120E-994B-B144-AC49F06A5BCE}" name="Spending or Income" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{5DA1230D-54BC-734B-A7E7-501E0542A11B}" name="Need/Want" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{B107A14D-0255-0149-B572-B678995ADF37}" name="Month" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{B38D5AA0-A0B8-E54B-84D7-E0C0E1511AE4}" name="Workday/Extended Weekend (inc Friday)" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{31B2C3DA-4854-9844-9496-96146F16A89E}" name="Method" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{F71D2D76-F449-6846-A86A-31D132D01864}" name="Transaction Date" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{698BE150-94AA-6647-A4A5-F0D1632492E8}" name="Category" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{62EA866A-6213-BE46-A5CC-E8DAC9C406A8}" name="Merchant" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{28935B6D-449E-5A45-AA26-1E8220AE2B4F}" name="Amount ($)" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{FD1C89E1-120E-994B-B144-AC49F06A5BCE}" name="Spending or Income" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{5DA1230D-54BC-734B-A7E7-501E0542A11B}" name="Need/Want" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{B107A14D-0255-0149-B572-B678995ADF37}" name="Month" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{B38D5AA0-A0B8-E54B-84D7-E0C0E1511AE4}" name="Workday/Extended Weekend (inc Friday)" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E0EF351-E274-B742-BA70-BF66AF535AA2}" name="clean_table" displayName="clean_table" ref="A1:I247" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E0EF351-E274-B742-BA70-BF66AF535AA2}" name="clean_table" displayName="clean_table" ref="A1:I247" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="A1:I247" xr:uid="{2E0EF351-E274-B742-BA70-BF66AF535AA2}">
     <filterColumn colId="2">
       <filters>
@@ -13508,18 +13602,18 @@
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A3AC953F-C3BF-EC4D-BED6-3CD2101D70CB}" name="Method"/>
-    <tableColumn id="2" xr3:uid="{A5BF0BD9-2C81-0044-A20C-49D5AAB02C7F}" name="Transaction Date" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{A5BF0BD9-2C81-0044-A20C-49D5AAB02C7F}" name="Transaction Date" dataDxfId="16"/>
     <tableColumn id="3" xr3:uid="{1F839404-3984-5942-A4B6-A0BA5517ECBE}" name="Category"/>
     <tableColumn id="4" xr3:uid="{2E492010-3649-CE4D-B40E-51953B8AA2B4}" name="Merchant"/>
     <tableColumn id="5" xr3:uid="{DA92C096-E88D-5247-9AFF-65920543CDCF}" name="Amount ($)"/>
-    <tableColumn id="9" xr3:uid="{7C9899EE-AB63-5148-93CF-F8AFDDB6142C}" name="Spending or Income" dataDxfId="5">
+    <tableColumn id="9" xr3:uid="{7C9899EE-AB63-5148-93CF-F8AFDDB6142C}" name="Spending or Income" dataDxfId="15">
       <calculatedColumnFormula>IF(clean_table[[#This Row],[Amount ($)]]&lt;0, "Spending", "Income")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{F75F65BF-D5DF-BB45-A978-62BAC39848E0}" name="Need/Want"/>
-    <tableColumn id="7" xr3:uid="{AD3A5953-37D8-9346-8570-AF420D890048}" name="Month" dataDxfId="4">
+    <tableColumn id="7" xr3:uid="{AD3A5953-37D8-9346-8570-AF420D890048}" name="Month" dataDxfId="14">
       <calculatedColumnFormula>TEXT(clean_table[[#This Row],[Transaction Date]], "mmmm")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2C48890E-6BA1-834F-8B9C-C6D4CD51ADFD}" name="Workday/Extended Weekend (inc Friday)" dataDxfId="3">
+    <tableColumn id="8" xr3:uid="{2C48890E-6BA1-834F-8B9C-C6D4CD51ADFD}" name="Workday/Extended Weekend (inc Friday)" dataDxfId="13">
       <calculatedColumnFormula>IF(WEEKDAY(clean_table[[#This Row],[Transaction Date]], 2) &lt;= 4, "Workday", "Ext-Weekend")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13804,8 +13898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40DA4593-1015-0D49-97A1-B65149B47EFD}">
   <dimension ref="A2:L24"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A16" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13872,19 +13966,28 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="52" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B20" s="42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="B23" s="43" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="23" x14ac:dyDescent="0.25">
-      <c r="B20" s="55" t="s">
+    <row r="24" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="A24" s="39"/>
+      <c r="B24" s="55" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="39"/>
-    </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -13894,7 +13997,7 @@
   <dimension ref="A2:K19"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="137" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14189,7 +14292,7 @@
   <dimension ref="A1:I247"/>
   <sheetViews>
     <sheetView zoomScale="138" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14200,7 +14303,7 @@
     <col min="4" max="4" width="16.5" customWidth="1"/>
     <col min="5" max="5" width="14.83203125" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="11.5" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
     <col min="9" max="9" width="38.33203125" customWidth="1"/>
   </cols>
@@ -22107,6 +22210,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -22156,7 +22260,7 @@
       <c r="A4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="57">
         <v>-1065.02</v>
       </c>
       <c r="D4" t="str">
@@ -22170,7 +22274,7 @@
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="57">
         <v>-929.1</v>
       </c>
       <c r="D5" t="str">
@@ -22184,7 +22288,7 @@
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="57">
         <v>-751.5</v>
       </c>
       <c r="D6" t="str">
@@ -22198,7 +22302,7 @@
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="57">
         <v>-474.3300000000001</v>
       </c>
       <c r="D7" t="str">
@@ -22212,7 +22316,7 @@
       <c r="A8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="57">
         <v>-240.11</v>
       </c>
       <c r="D8" t="str">
@@ -22226,7 +22330,7 @@
       <c r="A9" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="57">
         <v>-146.88999999999999</v>
       </c>
       <c r="D9" t="str">
@@ -22240,7 +22344,7 @@
       <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="57">
         <v>-140</v>
       </c>
       <c r="D10" t="str">
@@ -22254,7 +22358,7 @@
       <c r="A11" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="57">
         <v>-42.26</v>
       </c>
       <c r="D11" t="str">
@@ -22268,7 +22372,7 @@
       <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="57">
         <v>-33.9</v>
       </c>
       <c r="D12" t="str">
@@ -22282,7 +22386,7 @@
       <c r="A13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="57">
         <v>-9.24</v>
       </c>
     </row>
@@ -22290,7 +22394,7 @@
       <c r="A14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="57">
         <v>-2.99</v>
       </c>
     </row>
@@ -22298,16 +22402,16 @@
       <c r="A15" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="57">
         <v>-3835.3399999999997</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:A13">
-    <cfRule type="top10" dxfId="2" priority="1" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="12" priority="1" bottom="1" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="top10" dxfId="1" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="11" priority="2" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22339,7 +22443,7 @@
       <c r="A4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="57">
         <v>-575</v>
       </c>
     </row>
@@ -22347,7 +22451,7 @@
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="57">
         <v>-231.44</v>
       </c>
     </row>
@@ -22355,7 +22459,7 @@
       <c r="A6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="57">
         <v>-208.32999999999998</v>
       </c>
     </row>
@@ -22363,7 +22467,7 @@
       <c r="A7" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="57">
         <v>-170</v>
       </c>
     </row>
@@ -22371,7 +22475,7 @@
       <c r="A8" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="57">
         <v>-128.13</v>
       </c>
     </row>
@@ -22379,7 +22483,7 @@
       <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="57">
         <v>-111.64999999999998</v>
       </c>
     </row>
@@ -22387,7 +22491,7 @@
       <c r="A10" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="57">
         <v>-101.69</v>
       </c>
     </row>
@@ -22395,7 +22499,7 @@
       <c r="A11" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="57">
         <v>-86.37</v>
       </c>
     </row>
@@ -22403,7 +22507,7 @@
       <c r="A12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="57">
         <v>-84.22999999999999</v>
       </c>
     </row>
@@ -22411,7 +22515,7 @@
       <c r="A13" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="57">
         <v>-73.36</v>
       </c>
     </row>
@@ -22419,7 +22523,7 @@
       <c r="A14" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="57">
         <v>-67.48</v>
       </c>
     </row>
@@ -22427,7 +22531,7 @@
       <c r="A15" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="57">
         <v>-56.65</v>
       </c>
     </row>
@@ -22435,7 +22539,7 @@
       <c r="A16" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="57">
         <v>-53.56</v>
       </c>
     </row>
@@ -22443,7 +22547,7 @@
       <c r="A17" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="57">
         <v>-53.34</v>
       </c>
     </row>
@@ -22451,7 +22555,7 @@
       <c r="A18" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="57">
         <v>-51.02</v>
       </c>
     </row>
@@ -22459,7 +22563,7 @@
       <c r="A19" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="57">
         <v>-49.72</v>
       </c>
     </row>
@@ -22467,7 +22571,7 @@
       <c r="A20" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="57">
         <v>-48.300000000000004</v>
       </c>
     </row>
@@ -22475,7 +22579,7 @@
       <c r="A21" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="57">
         <v>-46.43</v>
       </c>
     </row>
@@ -22483,7 +22587,7 @@
       <c r="A22" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="57">
         <v>-45.2</v>
       </c>
     </row>
@@ -22491,7 +22595,7 @@
       <c r="A23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="57">
         <v>-36.21</v>
       </c>
     </row>
@@ -22499,7 +22603,7 @@
       <c r="A24" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="57">
         <v>-34.450000000000003</v>
       </c>
     </row>
@@ -22507,7 +22611,7 @@
       <c r="A25" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="57">
         <v>-33.9</v>
       </c>
     </row>
@@ -22515,7 +22619,7 @@
       <c r="A26" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="57">
         <v>-33.9</v>
       </c>
     </row>
@@ -22523,7 +22627,7 @@
       <c r="A27" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="57">
         <v>-33.880000000000003</v>
       </c>
     </row>
@@ -22531,7 +22635,7 @@
       <c r="A28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="57">
         <v>-31.830000000000002</v>
       </c>
     </row>
@@ -22539,7 +22643,7 @@
       <c r="A29" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="57">
         <v>-24.26</v>
       </c>
     </row>
@@ -22547,7 +22651,7 @@
       <c r="A30" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="57">
         <v>-22.6</v>
       </c>
     </row>
@@ -22555,7 +22659,7 @@
       <c r="A31" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="57">
         <v>-21.840000000000003</v>
       </c>
     </row>
@@ -22563,7 +22667,7 @@
       <c r="A32" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="57">
         <v>-20.11</v>
       </c>
     </row>
@@ -22571,7 +22675,7 @@
       <c r="A33" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="57">
         <v>-16.940000000000001</v>
       </c>
     </row>
@@ -22579,7 +22683,7 @@
       <c r="A34" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="57">
         <v>-16.100000000000001</v>
       </c>
     </row>
@@ -22587,7 +22691,7 @@
       <c r="A35" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="57">
         <v>-15.8</v>
       </c>
     </row>
@@ -22595,7 +22699,7 @@
       <c r="A36" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="57">
         <v>-15.18</v>
       </c>
     </row>
@@ -22603,7 +22707,7 @@
       <c r="A37" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="57">
         <v>-14.38</v>
       </c>
     </row>
@@ -22611,7 +22715,7 @@
       <c r="A38" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="57">
         <v>-14.16</v>
       </c>
     </row>
@@ -22619,7 +22723,7 @@
       <c r="A39" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="57">
         <v>-10.46</v>
       </c>
     </row>
@@ -22627,7 +22731,7 @@
       <c r="A40" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="57">
         <v>-10.17</v>
       </c>
     </row>
@@ -22635,7 +22739,7 @@
       <c r="A41" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="57">
         <v>-4.5999999999999996</v>
       </c>
     </row>
@@ -22643,7 +22747,7 @@
       <c r="A42" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="57">
         <v>-4.08</v>
       </c>
     </row>
@@ -22651,7 +22755,7 @@
       <c r="A43" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="57">
         <v>-2.99</v>
       </c>
     </row>
@@ -22659,7 +22763,7 @@
       <c r="A44" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="57">
         <v>4930.8200000000006</v>
       </c>
     </row>
@@ -22667,13 +22771,13 @@
       <c r="A45" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="57">
         <v>2271.0800000000004</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:A6">
-    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="10" priority="1" bottom="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37966,7 +38070,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83849630-1D1B-0441-A282-785374E7E158}">
   <dimension ref="A2:B9"/>
   <sheetViews>
-    <sheetView zoomScale="179" workbookViewId="0"/>
+    <sheetView zoomScale="179" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -38045,8 +38151,8 @@
   </sheetPr>
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38245,6 +38351,7 @@
       <c r="J33" s="26"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="B1:Q1"/>
   </mergeCells>
@@ -38271,158 +38378,224 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="151" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="59" t="s">
         <v>81</v>
       </c>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="59" t="s">
         <v>79</v>
       </c>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="59"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="58" t="s">
         <v>4</v>
       </c>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="59" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10">
+      <c r="B6" s="61"/>
+      <c r="C6" s="61">
         <v>1132.95</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="61">
         <v>44</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="61">
         <v>1176.95</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10">
+      <c r="B7" s="61"/>
+      <c r="C7" s="61">
         <v>1040.3900000000001</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="61">
         <v>332</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="61">
         <v>1372.39</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="61">
         <v>225</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="61">
         <v>2037.5</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="61">
         <v>765.72</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="61">
         <v>3028.2200000000003</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10">
+      <c r="B9" s="61"/>
+      <c r="C9" s="61">
         <v>723.73</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="61">
         <v>328.14</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="61">
         <v>1051.8699999999999</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="61">
         <v>225</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="61">
         <v>4934.57</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="61">
         <v>1469.8600000000001</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="61">
         <v>6629.43</v>
       </c>
     </row>
-    <row r="20" spans="7:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="59"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="59"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="59"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="59"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="59"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="59"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="59"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+    </row>
+    <row r="20" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="G20" s="48" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="7:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="G21" s="46"/>
     </row>
-    <row r="22" spans="7:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="G22" s="47" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="7:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="G23" s="47" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
   <extLst>

</xml_diff>

<commit_message>
Excel and Readme changes
</commit_message>
<xml_diff>
--- a/Money Matters/Money Matters.xlsx
+++ b/Money Matters/Money Matters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliangriffin/Desktop/NewExcel_Projects_Local/NewExcel_Projects/Money Matters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D010B88-72A0-9D46-B49A-873640319078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B94926-34AC-5B4C-A56E-B7FDC8096BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId13"/>
+    <pivotCache cacheId="2" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3122" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3121" uniqueCount="115">
   <si>
     <t>Method</t>
   </si>
@@ -1292,10 +1292,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1309,6 +1305,10 @@
     <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="3" builtinId="37"/>
@@ -1317,36 +1317,6 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{0CBFBBA0-2B04-F540-AA3A-5B59D7AB2613}"/>
   </cellStyles>
   <dxfs count="42">
-    <dxf>
-      <protection locked="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0"/>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1436,6 +1406,36 @@
       <font>
         <sz val="12"/>
       </font>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2870,13 +2870,13 @@
                   <c:v>-1032.8100000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-780.70999999999992</c:v>
+                  <c:v>-680.70999999999992</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>-1253.9899999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-767.83</c:v>
+                  <c:v>-727.83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3519,16 +3519,16 @@
                   <c:v>Clothing</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Withdrawal</c:v>
+                  <c:v>Fitness</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Fitness</c:v>
+                  <c:v>Gift</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Gift</c:v>
+                  <c:v>Other</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Other</c:v>
+                  <c:v>Grocery</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3558,16 +3558,16 @@
                   <c:v>146.88999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>140</c:v>
+                  <c:v>42.26</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42.26</c:v>
+                  <c:v>33.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33.9</c:v>
+                  <c:v>9.24</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.24</c:v>
+                  <c:v>2.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8370,8 +8370,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>226464</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="8" name="Category">
@@ -8394,7 +8394,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8448,8 +8448,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>148251</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:tsle="http://schemas.microsoft.com/office/drawing/2012/timeslicer" Requires="tsle">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:tsle="http://schemas.microsoft.com/office/drawing/2012/timeslicer">
+      <mc:Choice Requires="tsle">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="9" name="Transaction Date">
@@ -8467,12 +8467,12 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2012/timeslicer">
-              <tsle:timeslicer xmlns:tsle="http://schemas.microsoft.com/office/drawing/2012/timeslicer" name="Transaction Date"/>
+              <tsle:timeslicer name="Transaction Date"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8525,8 +8525,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>239037</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="10" name="Workday/Extended Weekend (inc Friday)">
@@ -8549,7 +8549,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8603,8 +8603,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>173398</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="11" name="Method">
@@ -8627,7 +8627,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8760,8 +8760,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Month">
@@ -8784,7 +8784,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -11882,8 +11882,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EB3F11B9-D113-7F4A-91F0-B3EFC801EA5E}" name="pivot_category" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EB3F11B9-D113-7F4A-91F0-B3EFC801EA5E}" name="pivot_category" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField showAll="0">
       <items count="3">
@@ -11994,7 +11994,7 @@
         <item x="13"/>
         <item h="1" x="15"/>
         <item x="1"/>
-        <item x="11"/>
+        <item h="1" x="11"/>
         <item t="default"/>
       </items>
       <autoSortScope>
@@ -12029,7 +12029,7 @@
   <rowFields count="1">
     <field x="2"/>
   </rowFields>
-  <rowItems count="12">
+  <rowItems count="11">
     <i>
       <x v="15"/>
     </i>
@@ -12047,9 +12047,6 @@
     </i>
     <i>
       <x v="2"/>
-    </i>
-    <i>
-      <x v="16"/>
     </i>
     <i>
       <x v="5"/>
@@ -12089,7 +12086,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{971C53EE-E45E-FF4C-955C-416D24A2441E}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{971C53EE-E45E-FF4C-955C-416D24A2441E}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B45" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0">
@@ -12201,7 +12198,7 @@
         <item x="13"/>
         <item h="1" x="15"/>
         <item x="1"/>
-        <item x="11"/>
+        <item h="1" x="11"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -12429,7 +12426,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4EE3A639-4420-FA42-BED3-A9AF713D5EBD}" name="expenses_table" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12" rowHeaderCaption="Category" colHeaderCaption="DOW">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4EE3A639-4420-FA42-BED3-A9AF713D5EBD}" name="expenses_table" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12" rowHeaderCaption="Category" colHeaderCaption="DOW">
   <location ref="A5:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisPage" showAll="0">
@@ -12525,7 +12522,7 @@
     </pivotField>
     <pivotField showAll="0" sortType="descending">
       <items count="18">
-        <item x="11"/>
+        <item h="1" x="11"/>
         <item x="1"/>
         <item h="1" x="15"/>
         <item x="13"/>
@@ -12635,7 +12632,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7DA7F608-522A-7B4A-A0D7-DCA332F361E7}" name="earnings_pivot" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="25" rowHeaderCaption="Category" colHeaderCaption="Month">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7DA7F608-522A-7B4A-A0D7-DCA332F361E7}" name="earnings_pivot" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="25" rowHeaderCaption="Category" colHeaderCaption="Month">
   <location ref="A4:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField showAll="0">
@@ -12747,7 +12744,7 @@
         <item sd="0" x="13"/>
         <item h="1" sd="0" x="15"/>
         <item x="1"/>
-        <item x="11"/>
+        <item h="1" x="11"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -12895,7 +12892,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{673BB614-F46B-1243-97E1-B14448CFB4EC}" name="earnings_pivot" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19" rowHeaderCaption="Category" colHeaderCaption="Month">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{673BB614-F46B-1243-97E1-B14448CFB4EC}" name="earnings_pivot" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19" rowHeaderCaption="Category" colHeaderCaption="Month">
   <location ref="A4:E10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisPage" showAll="0">
@@ -13046,35 +13043,35 @@
     <dataField name="Total Amount ($)" fld="4" baseField="0" baseItem="0" numFmtId="7"/>
   </dataFields>
   <formats count="10">
-    <format dxfId="0">
+    <format dxfId="20">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="19">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="18">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="17">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="16">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="15">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="7" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="3">
@@ -13085,7 +13082,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -13176,7 +13173,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D3F80AAA-42CD-A342-8A8D-09149152666B}" name="expenses_table" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11" rowHeaderCaption="Category" colHeaderCaption="DOW">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D3F80AAA-42CD-A342-8A8D-09149152666B}" name="expenses_table" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11" rowHeaderCaption="Category" colHeaderCaption="DOW">
   <location ref="A5:D18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisPage" showAll="0">
@@ -13291,7 +13288,7 @@
     <dataField name="Total Amount ($)" fld="4" baseField="0" baseItem="0" numFmtId="42"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="20">
+    <format dxfId="10">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -13408,7 +13405,7 @@
         <i x="13" s="1"/>
         <i x="15"/>
         <i x="1" s="1"/>
-        <i x="11" s="1"/>
+        <i x="11"/>
       </items>
     </tabular>
   </data>
@@ -13576,7 +13573,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E0EF351-E274-B742-BA70-BF66AF535AA2}" name="clean_table" displayName="clean_table" ref="A1:I247" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E0EF351-E274-B742-BA70-BF66AF535AA2}" name="clean_table" displayName="clean_table" ref="A1:I247" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A1:I247" xr:uid="{2E0EF351-E274-B742-BA70-BF66AF535AA2}">
     <filterColumn colId="2">
       <filters>
@@ -13602,18 +13599,18 @@
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A3AC953F-C3BF-EC4D-BED6-3CD2101D70CB}" name="Method"/>
-    <tableColumn id="2" xr3:uid="{A5BF0BD9-2C81-0044-A20C-49D5AAB02C7F}" name="Transaction Date" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{A5BF0BD9-2C81-0044-A20C-49D5AAB02C7F}" name="Transaction Date" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{1F839404-3984-5942-A4B6-A0BA5517ECBE}" name="Category"/>
     <tableColumn id="4" xr3:uid="{2E492010-3649-CE4D-B40E-51953B8AA2B4}" name="Merchant"/>
     <tableColumn id="5" xr3:uid="{DA92C096-E88D-5247-9AFF-65920543CDCF}" name="Amount ($)"/>
-    <tableColumn id="9" xr3:uid="{7C9899EE-AB63-5148-93CF-F8AFDDB6142C}" name="Spending or Income" dataDxfId="15">
+    <tableColumn id="9" xr3:uid="{7C9899EE-AB63-5148-93CF-F8AFDDB6142C}" name="Spending or Income" dataDxfId="5">
       <calculatedColumnFormula>IF(clean_table[[#This Row],[Amount ($)]]&lt;0, "Spending", "Income")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{F75F65BF-D5DF-BB45-A978-62BAC39848E0}" name="Need/Want"/>
-    <tableColumn id="7" xr3:uid="{AD3A5953-37D8-9346-8570-AF420D890048}" name="Month" dataDxfId="14">
+    <tableColumn id="7" xr3:uid="{AD3A5953-37D8-9346-8570-AF420D890048}" name="Month" dataDxfId="4">
       <calculatedColumnFormula>TEXT(clean_table[[#This Row],[Transaction Date]], "mmmm")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2C48890E-6BA1-834F-8B9C-C6D4CD51ADFD}" name="Workday/Extended Weekend (inc Friday)" dataDxfId="13">
+    <tableColumn id="8" xr3:uid="{2C48890E-6BA1-834F-8B9C-C6D4CD51ADFD}" name="Workday/Extended Weekend (inc Friday)" dataDxfId="3">
       <calculatedColumnFormula>IF(WEEKDAY(clean_table[[#This Row],[Transaction Date]], 2) &lt;= 4, "Workday", "Ext-Weekend")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13898,7 +13895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40DA4593-1015-0D49-97A1-B65149B47EFD}">
   <dimension ref="A2:L24"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="114" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="114" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -13997,7 +13994,7 @@
   <dimension ref="A2:K19"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="137" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14292,7 +14289,7 @@
   <dimension ref="A1:I247"/>
   <sheetViews>
     <sheetView zoomScale="138" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22220,7 +22217,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B813E8-23BF-FF44-B015-1FE81D517B4E}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScale="172" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
@@ -22260,7 +22257,7 @@
       <c r="A4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="57">
+      <c r="B4" s="61">
         <v>-1065.02</v>
       </c>
       <c r="D4" t="str">
@@ -22274,7 +22271,7 @@
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="57">
+      <c r="B5" s="61">
         <v>-929.1</v>
       </c>
       <c r="D5" t="str">
@@ -22288,7 +22285,7 @@
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="57">
+      <c r="B6" s="61">
         <v>-751.5</v>
       </c>
       <c r="D6" t="str">
@@ -22302,7 +22299,7 @@
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="57">
+      <c r="B7" s="61">
         <v>-474.3300000000001</v>
       </c>
       <c r="D7" t="str">
@@ -22316,7 +22313,7 @@
       <c r="A8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="57">
+      <c r="B8" s="61">
         <v>-240.11</v>
       </c>
       <c r="D8" t="str">
@@ -22330,88 +22327,80 @@
       <c r="A9" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="57">
+      <c r="B9" s="61">
         <v>-146.88999999999999</v>
       </c>
       <c r="D9" t="str">
-        <v>Withdrawal</v>
+        <v>Fitness</v>
       </c>
       <c r="E9">
-        <v>140</v>
+        <v>42.26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="57">
-        <v>-140</v>
+        <v>44</v>
+      </c>
+      <c r="B10" s="61">
+        <v>-42.26</v>
       </c>
       <c r="D10" t="str">
-        <v>Fitness</v>
+        <v>Gift</v>
       </c>
       <c r="E10">
-        <v>42.26</v>
+        <v>33.9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="57">
-        <v>-42.26</v>
+        <v>20</v>
+      </c>
+      <c r="B11" s="61">
+        <v>-33.9</v>
       </c>
       <c r="D11" t="str">
-        <v>Gift</v>
+        <v>Other</v>
       </c>
       <c r="E11">
-        <v>33.9</v>
+        <v>9.24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="57">
-        <v>-33.9</v>
+        <v>30</v>
+      </c>
+      <c r="B12" s="61">
+        <v>-9.24</v>
       </c>
       <c r="D12" t="str">
-        <v>Other</v>
+        <v>Grocery</v>
       </c>
       <c r="E12">
-        <v>9.24</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="57">
-        <v>-9.24</v>
+        <v>37</v>
+      </c>
+      <c r="B13" s="61">
+        <v>-2.99</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="57">
-        <v>-2.99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="57">
-        <v>-3835.3399999999997</v>
+      <c r="B14" s="61">
+        <v>-3695.3399999999997</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:A13">
-    <cfRule type="top10" dxfId="12" priority="1" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="2" priority="1" bottom="1" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="top10" dxfId="11" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="1" priority="2" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22443,7 +22432,7 @@
       <c r="A4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="57">
+      <c r="B4" s="61">
         <v>-575</v>
       </c>
     </row>
@@ -22451,7 +22440,7 @@
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="57">
+      <c r="B5" s="61">
         <v>-231.44</v>
       </c>
     </row>
@@ -22459,7 +22448,7 @@
       <c r="A6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="57">
+      <c r="B6" s="61">
         <v>-208.32999999999998</v>
       </c>
     </row>
@@ -22467,7 +22456,7 @@
       <c r="A7" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="57">
+      <c r="B7" s="61">
         <v>-170</v>
       </c>
     </row>
@@ -22475,7 +22464,7 @@
       <c r="A8" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="57">
+      <c r="B8" s="61">
         <v>-128.13</v>
       </c>
     </row>
@@ -22483,7 +22472,7 @@
       <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="57">
+      <c r="B9" s="61">
         <v>-111.64999999999998</v>
       </c>
     </row>
@@ -22491,7 +22480,7 @@
       <c r="A10" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="57">
+      <c r="B10" s="61">
         <v>-101.69</v>
       </c>
     </row>
@@ -22499,7 +22488,7 @@
       <c r="A11" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="57">
+      <c r="B11" s="61">
         <v>-86.37</v>
       </c>
     </row>
@@ -22507,7 +22496,7 @@
       <c r="A12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="57">
+      <c r="B12" s="61">
         <v>-84.22999999999999</v>
       </c>
     </row>
@@ -22515,7 +22504,7 @@
       <c r="A13" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="57">
+      <c r="B13" s="61">
         <v>-73.36</v>
       </c>
     </row>
@@ -22523,7 +22512,7 @@
       <c r="A14" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="57">
+      <c r="B14" s="61">
         <v>-67.48</v>
       </c>
     </row>
@@ -22531,7 +22520,7 @@
       <c r="A15" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="57">
+      <c r="B15" s="61">
         <v>-56.65</v>
       </c>
     </row>
@@ -22539,7 +22528,7 @@
       <c r="A16" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="57">
+      <c r="B16" s="61">
         <v>-53.56</v>
       </c>
     </row>
@@ -22547,7 +22536,7 @@
       <c r="A17" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="57">
+      <c r="B17" s="61">
         <v>-53.34</v>
       </c>
     </row>
@@ -22555,7 +22544,7 @@
       <c r="A18" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="57">
+      <c r="B18" s="61">
         <v>-51.02</v>
       </c>
     </row>
@@ -22563,7 +22552,7 @@
       <c r="A19" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="57">
+      <c r="B19" s="61">
         <v>-49.72</v>
       </c>
     </row>
@@ -22571,7 +22560,7 @@
       <c r="A20" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="57">
+      <c r="B20" s="61">
         <v>-48.300000000000004</v>
       </c>
     </row>
@@ -22579,7 +22568,7 @@
       <c r="A21" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="57">
+      <c r="B21" s="61">
         <v>-46.43</v>
       </c>
     </row>
@@ -22587,7 +22576,7 @@
       <c r="A22" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="57">
+      <c r="B22" s="61">
         <v>-45.2</v>
       </c>
     </row>
@@ -22595,7 +22584,7 @@
       <c r="A23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="57">
+      <c r="B23" s="61">
         <v>-36.21</v>
       </c>
     </row>
@@ -22603,7 +22592,7 @@
       <c r="A24" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="57">
+      <c r="B24" s="61">
         <v>-34.450000000000003</v>
       </c>
     </row>
@@ -22611,7 +22600,7 @@
       <c r="A25" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="57">
+      <c r="B25" s="61">
         <v>-33.9</v>
       </c>
     </row>
@@ -22619,7 +22608,7 @@
       <c r="A26" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="57">
+      <c r="B26" s="61">
         <v>-33.9</v>
       </c>
     </row>
@@ -22627,7 +22616,7 @@
       <c r="A27" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="57">
+      <c r="B27" s="61">
         <v>-33.880000000000003</v>
       </c>
     </row>
@@ -22635,7 +22624,7 @@
       <c r="A28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="57">
+      <c r="B28" s="61">
         <v>-31.830000000000002</v>
       </c>
     </row>
@@ -22643,7 +22632,7 @@
       <c r="A29" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="57">
+      <c r="B29" s="61">
         <v>-24.26</v>
       </c>
     </row>
@@ -22651,7 +22640,7 @@
       <c r="A30" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="57">
+      <c r="B30" s="61">
         <v>-22.6</v>
       </c>
     </row>
@@ -22659,7 +22648,7 @@
       <c r="A31" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="57">
+      <c r="B31" s="61">
         <v>-21.840000000000003</v>
       </c>
     </row>
@@ -22667,7 +22656,7 @@
       <c r="A32" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="57">
+      <c r="B32" s="61">
         <v>-20.11</v>
       </c>
     </row>
@@ -22675,7 +22664,7 @@
       <c r="A33" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="57">
+      <c r="B33" s="61">
         <v>-16.940000000000001</v>
       </c>
     </row>
@@ -22683,7 +22672,7 @@
       <c r="A34" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="57">
+      <c r="B34" s="61">
         <v>-16.100000000000001</v>
       </c>
     </row>
@@ -22691,7 +22680,7 @@
       <c r="A35" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="57">
+      <c r="B35" s="61">
         <v>-15.8</v>
       </c>
     </row>
@@ -22699,7 +22688,7 @@
       <c r="A36" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="57">
+      <c r="B36" s="61">
         <v>-15.18</v>
       </c>
     </row>
@@ -22707,7 +22696,7 @@
       <c r="A37" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="57">
+      <c r="B37" s="61">
         <v>-14.38</v>
       </c>
     </row>
@@ -22715,7 +22704,7 @@
       <c r="A38" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B38" s="57">
+      <c r="B38" s="61">
         <v>-14.16</v>
       </c>
     </row>
@@ -22723,7 +22712,7 @@
       <c r="A39" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="57">
+      <c r="B39" s="61">
         <v>-10.46</v>
       </c>
     </row>
@@ -22731,7 +22720,7 @@
       <c r="A40" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="57">
+      <c r="B40" s="61">
         <v>-10.17</v>
       </c>
     </row>
@@ -22739,7 +22728,7 @@
       <c r="A41" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="57">
+      <c r="B41" s="61">
         <v>-4.5999999999999996</v>
       </c>
     </row>
@@ -22747,7 +22736,7 @@
       <c r="A42" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="57">
+      <c r="B42" s="61">
         <v>-4.08</v>
       </c>
     </row>
@@ -22755,7 +22744,7 @@
       <c r="A43" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="57">
+      <c r="B43" s="61">
         <v>-2.99</v>
       </c>
     </row>
@@ -22763,7 +22752,7 @@
       <c r="A44" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B44" s="57">
+      <c r="B44" s="61">
         <v>4930.8200000000006</v>
       </c>
     </row>
@@ -22771,13 +22760,13 @@
       <c r="A45" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="57">
+      <c r="B45" s="61">
         <v>2271.0800000000004</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:A6">
-    <cfRule type="top10" dxfId="10" priority="1" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37976,7 +37965,7 @@
         <v>75</v>
       </c>
       <c r="B7" s="9">
-        <v>-780.70999999999992</v>
+        <v>-680.70999999999992</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="2"/>
@@ -37998,7 +37987,7 @@
         <v>77</v>
       </c>
       <c r="B9" s="9">
-        <v>-767.83</v>
+        <v>-727.83</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="2"/>
@@ -38009,7 +37998,7 @@
         <v>78</v>
       </c>
       <c r="B10" s="9">
-        <v>-3835.3399999999992</v>
+        <v>-3695.3399999999992</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="2"/>
@@ -38151,7 +38140,7 @@
   </sheetPr>
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -38168,24 +38157,24 @@
   <sheetData>
     <row r="1" spans="1:17" ht="59" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
@@ -38234,7 +38223,7 @@
       </c>
       <c r="I11" s="27">
         <f>GETPIVOTDATA("Amount ($)",PivotExpenses_Chart!$A$5)</f>
-        <v>-3835.3399999999992</v>
+        <v>-3695.3399999999992</v>
       </c>
       <c r="J11" s="25"/>
     </row>
@@ -38256,7 +38245,7 @@
       </c>
       <c r="I13" s="29">
         <f>I12+I11</f>
-        <v>2119.09</v>
+        <v>2259.09</v>
       </c>
       <c r="J13" s="25"/>
     </row>
@@ -38378,7 +38367,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="151" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -38392,189 +38381,189 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="59" t="s">
+      <c r="A2" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="59"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="57" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61">
+      <c r="B6" s="59"/>
+      <c r="C6" s="59">
         <v>1132.95</v>
       </c>
-      <c r="D6" s="61">
+      <c r="D6" s="59">
         <v>44</v>
       </c>
-      <c r="E6" s="61">
+      <c r="E6" s="59">
         <v>1176.95</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61">
+      <c r="B7" s="59"/>
+      <c r="C7" s="59">
         <v>1040.3900000000001</v>
       </c>
-      <c r="D7" s="61">
+      <c r="D7" s="59">
         <v>332</v>
       </c>
-      <c r="E7" s="61">
+      <c r="E7" s="59">
         <v>1372.39</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="61">
+      <c r="B8" s="59">
         <v>225</v>
       </c>
-      <c r="C8" s="61">
+      <c r="C8" s="59">
         <v>2037.5</v>
       </c>
-      <c r="D8" s="61">
+      <c r="D8" s="59">
         <v>765.72</v>
       </c>
-      <c r="E8" s="61">
+      <c r="E8" s="59">
         <v>3028.2200000000003</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61">
+      <c r="B9" s="59"/>
+      <c r="C9" s="59">
         <v>723.73</v>
       </c>
-      <c r="D9" s="61">
+      <c r="D9" s="59">
         <v>328.14</v>
       </c>
-      <c r="E9" s="61">
+      <c r="E9" s="59">
         <v>1051.8699999999999</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="61">
+      <c r="B10" s="59">
         <v>225</v>
       </c>
-      <c r="C10" s="61">
+      <c r="C10" s="59">
         <v>4934.57</v>
       </c>
-      <c r="D10" s="61">
+      <c r="D10" s="59">
         <v>1469.8600000000001</v>
       </c>
-      <c r="E10" s="61">
+      <c r="E10" s="59">
         <v>6629.43</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="59"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="59"/>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="59"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="59"/>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="59"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="59"/>
-      <c r="B16" s="59"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="59"/>
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
     </row>
     <row r="20" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="G20" s="48" t="s">

</xml_diff>

<commit_message>
Gif changes and protections
</commit_message>
<xml_diff>
--- a/Money Matters/Money Matters.xlsx
+++ b/Money Matters/Money Matters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliangriffin/Desktop/NewExcel_Projects_Local/NewExcel_Projects/Money Matters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B94926-34AC-5B4C-A56E-B7FDC8096BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0395AAE-F2F3-F44F-ABCF-C628F5456735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId13"/>
+    <pivotCache cacheId="1" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3121" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3115" uniqueCount="115">
   <si>
     <t>Method</t>
   </si>
@@ -397,9 +397,6 @@
   </si>
   <si>
     <t>Talk soon,</t>
-  </si>
-  <si>
-    <t>CLICK ME !! &gt;&gt;&gt;&gt;</t>
   </si>
   <si>
     <t>What is this?</t>
@@ -736,6 +733,9 @@
   <si>
     <t>The sheet is protected so only the slicers and chart fields are avalable for change.</t>
   </si>
+  <si>
+    <t>CLICK ME</t>
+  </si>
 </sst>
 </file>
 
@@ -914,13 +914,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="36"/>
-      <color theme="1"/>
-      <name val="Gill Sans MT"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
@@ -977,6 +970,11 @@
       <name val="Gill Sans MT"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Gill Sans MT (Body)"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1225,7 +1223,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -1272,26 +1270,19 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1308,7 +1299,20 @@
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="3" builtinId="37"/>
@@ -1316,7 +1320,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{0CBFBBA0-2B04-F540-AA3A-5B59D7AB2613}"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="45">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1346,6 +1350,20 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1401,11 +1419,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
     </dxf>
     <dxf>
       <protection locked="0"/>
@@ -2867,16 +2880,16 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-1032.8100000000002</c:v>
+                  <c:v>-765.30000000000018</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-680.70999999999992</c:v>
+                  <c:v>-535.68000000000006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1253.9899999999996</c:v>
+                  <c:v>-841.40000000000009</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-727.83</c:v>
+                  <c:v>-487.93999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3501,34 +3514,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Transportation</c:v>
+                  <c:v>Entertainment</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Entertainment</c:v>
+                  <c:v>E-Transfer</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>E-Transfer</c:v>
+                  <c:v>Food</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Food</c:v>
+                  <c:v>Healthcare</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Healthcare</c:v>
+                  <c:v>Clothing</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Clothing</c:v>
+                  <c:v>Fitness</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Fitness</c:v>
+                  <c:v>Gift</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Gift</c:v>
+                  <c:v>Other</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Other</c:v>
+                  <c:v>Grocery</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Grocery</c:v>
+                  <c:v>Grand Total</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3540,34 +3553,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1065.02</c:v>
+                  <c:v>929.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>929.1</c:v>
+                  <c:v>751.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>751.5</c:v>
+                  <c:v>474.33000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>474.3300000000001</c:v>
+                  <c:v>240.11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>240.11</c:v>
+                  <c:v>146.88999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>146.88999999999999</c:v>
+                  <c:v>42.26</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42.26</c:v>
+                  <c:v>33.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33.9</c:v>
+                  <c:v>9.24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.24</c:v>
+                  <c:v>2.99</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.99</c:v>
+                  <c:v>2630.3199999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4484,7 +4497,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-21FF-3C48-9C68-58BEE80C1D24}"/>
+              <c16:uniqueId val="{00000003-BB4B-E545-A9F1-4037DD7E540E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4940,7 +4953,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Pivot_Expenses!$B$5:$B$6</c:f>
+              <c:f>Pivot_Expenses!$C$7:$C$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5057,7 +5070,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Pivot_Expenses!$A$7:$A$18</c:f>
+              <c:f>Pivot_Expenses!$B$9:$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -5098,7 +5111,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pivot_Expenses!$B$7:$B$18</c:f>
+              <c:f>Pivot_Expenses!$C$9:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5140,7 +5153,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Pivot_Expenses!$C$5:$C$6</c:f>
+              <c:f>Pivot_Expenses!$D$7:$D$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5257,7 +5270,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Pivot_Expenses!$A$7:$A$18</c:f>
+              <c:f>Pivot_Expenses!$B$9:$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -5298,7 +5311,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pivot_Expenses!$C$7:$C$18</c:f>
+              <c:f>Pivot_Expenses!$D$9:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5331,7 +5344,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-4242-8448-93F1-E633E356EB81}"/>
+              <c16:uniqueId val="{00000004-8FBD-9B44-98D0-4B37A18187B0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8672,8 +8685,8 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>12575</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>292099</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2891</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
@@ -8704,6 +8717,77 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>520700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Right Arrow 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB39C56A-8047-4F39-FD5D-946589A43045}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3124200" y="2070100"/>
+          <a:ext cx="1308100" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -8832,16 +8916,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1927</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3403</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>200568</xdr:rowOff>
+      <xdr:rowOff>191090</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>509854</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>247804</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>57400</xdr:rowOff>
+      <xdr:rowOff>47922</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8869,18 +8953,18 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>13083</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>1540</xdr:rowOff>
+      <xdr:colOff>299857</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>155168</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>240528</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>234705</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>125076</xdr:rowOff>
+      <xdr:rowOff>84108</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Workday/Extended Weekend (inc Friday) 1">
@@ -8903,7 +8987,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8913,8 +8997,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4879871" y="5350372"/>
-              <a:ext cx="5057153" cy="902222"/>
+              <a:off x="5192653" y="5303031"/>
+              <a:ext cx="5056632" cy="898405"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -8942,7 +9026,7 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
-    <xdr:clientData/>
+    <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
@@ -11882,8 +11966,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EB3F11B9-D113-7F4A-91F0-B3EFC801EA5E}" name="pivot_category" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EB3F11B9-D113-7F4A-91F0-B3EFC801EA5E}" name="pivot_category" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="A3:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField showAll="0">
       <items count="3">
@@ -11993,7 +12077,7 @@
         <item h="1" x="5"/>
         <item x="13"/>
         <item h="1" x="15"/>
-        <item x="1"/>
+        <item h="1" x="1"/>
         <item h="1" x="11"/>
         <item t="default"/>
       </items>
@@ -12029,10 +12113,7 @@
   <rowFields count="1">
     <field x="2"/>
   </rowFields>
-  <rowItems count="11">
-    <i>
-      <x v="15"/>
-    </i>
+  <rowItems count="10">
     <i>
       <x v="4"/>
     </i>
@@ -12086,8 +12167,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{971C53EE-E45E-FF4C-955C-416D24A2441E}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B45" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{971C53EE-E45E-FF4C-955C-416D24A2441E}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B40" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0">
       <items count="3">
@@ -12197,7 +12278,7 @@
         <item h="1" x="5"/>
         <item x="13"/>
         <item h="1" x="15"/>
-        <item x="1"/>
+        <item h="1" x="1"/>
         <item h="1" x="11"/>
         <item t="default"/>
       </items>
@@ -12279,16 +12360,7 @@
   <rowFields count="1">
     <field x="3"/>
   </rowFields>
-  <rowItems count="42">
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
+  <rowItems count="37">
     <i>
       <x v="43"/>
     </i>
@@ -12341,13 +12413,10 @@
       <x v="39"/>
     </i>
     <i>
-      <x v="38"/>
+      <x v="26"/>
     </i>
     <i>
       <x v="31"/>
-    </i>
-    <i>
-      <x v="26"/>
     </i>
     <i>
       <x v="35"/>
@@ -12372,9 +12441,6 @@
     </i>
     <i>
       <x v="4"/>
-    </i>
-    <i>
-      <x v="29"/>
     </i>
     <i>
       <x v="41"/>
@@ -12426,7 +12492,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4EE3A639-4420-FA42-BED3-A9AF713D5EBD}" name="expenses_table" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12" rowHeaderCaption="Category" colHeaderCaption="DOW">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4EE3A639-4420-FA42-BED3-A9AF713D5EBD}" name="expenses_table" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12" rowHeaderCaption="Category" colHeaderCaption="DOW">
   <location ref="A5:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisPage" showAll="0">
@@ -12523,7 +12589,7 @@
     <pivotField showAll="0" sortType="descending">
       <items count="18">
         <item h="1" x="11"/>
-        <item x="1"/>
+        <item h="1" x="1"/>
         <item h="1" x="15"/>
         <item x="13"/>
         <item h="1" x="5"/>
@@ -12632,7 +12698,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7DA7F608-522A-7B4A-A0D7-DCA332F361E7}" name="earnings_pivot" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="25" rowHeaderCaption="Category" colHeaderCaption="Month">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7DA7F608-522A-7B4A-A0D7-DCA332F361E7}" name="earnings_pivot" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="25" rowHeaderCaption="Category" colHeaderCaption="Month">
   <location ref="A4:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField showAll="0">
@@ -12743,7 +12809,7 @@
         <item h="1" x="5"/>
         <item sd="0" x="13"/>
         <item h="1" sd="0" x="15"/>
-        <item x="1"/>
+        <item h="1" x="1"/>
         <item h="1" x="11"/>
         <item t="default"/>
       </items>
@@ -12892,7 +12958,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{673BB614-F46B-1243-97E1-B14448CFB4EC}" name="earnings_pivot" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19" rowHeaderCaption="Category" colHeaderCaption="Month">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{673BB614-F46B-1243-97E1-B14448CFB4EC}" name="earnings_pivot" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19" rowHeaderCaption="Category" colHeaderCaption="Month">
   <location ref="A4:E10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisPage" showAll="0">
@@ -13043,35 +13109,35 @@
     <dataField name="Total Amount ($)" fld="4" baseField="0" baseItem="0" numFmtId="7"/>
   </dataFields>
   <formats count="10">
-    <format dxfId="20">
+    <format dxfId="23">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="22">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="18">
+    <format dxfId="21">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="20">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="19">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="18">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="14">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="7" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="3">
@@ -13082,7 +13148,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -13173,8 +13239,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D3F80AAA-42CD-A342-8A8D-09149152666B}" name="expenses_table" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11" rowHeaderCaption="Category" colHeaderCaption="DOW">
-  <location ref="A5:D18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D3F80AAA-42CD-A342-8A8D-09149152666B}" name="expenses_table" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11" rowHeaderCaption="Category" colHeaderCaption="DOW">
+  <location ref="B7:E20" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisPage" showAll="0">
       <items count="3">
@@ -13287,9 +13353,38 @@
   <dataFields count="1">
     <dataField name="Total Amount ($)" fld="4" baseField="0" baseItem="0" numFmtId="42"/>
   </dataFields>
-  <formats count="1">
-    <format dxfId="10">
+  <formats count="4">
+    <format dxfId="6">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="5">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="11">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+            <x v="13"/>
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="8" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
   <chartFormats count="6">
@@ -13391,12 +13486,10 @@
       <items count="17">
         <i x="9"/>
         <i x="6"/>
-        <i x="16" s="1"/>
         <i x="0" s="1"/>
         <i x="3" s="1"/>
         <i x="14" s="1"/>
         <i x="2" s="1"/>
-        <i x="7" s="1"/>
         <i x="12" s="1"/>
         <i x="8" s="1"/>
         <i x="10" s="1"/>
@@ -13404,8 +13497,10 @@
         <i x="5"/>
         <i x="13" s="1"/>
         <i x="15"/>
-        <i x="1" s="1"/>
+        <i x="1"/>
         <i x="11"/>
+        <i x="16" s="1" nd="1"/>
+        <i x="7" s="1" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -13509,7 +13604,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1CE2BBCA-3F43-EA48-9EC4-0007134C9FBC}" name="expenses_table" displayName="expenses_table" ref="A1:I247" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1CE2BBCA-3F43-EA48-9EC4-0007134C9FBC}" name="expenses_table" displayName="expenses_table" ref="A1:I247" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42">
   <autoFilter ref="A1:I247" xr:uid="{1CE2BBCA-3F43-EA48-9EC4-0007134C9FBC}">
     <filterColumn colId="4">
       <customFilters>
@@ -13522,18 +13617,18 @@
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F10CA1B2-7120-C84C-8023-87180B21085B}" name="Method"/>
-    <tableColumn id="2" xr3:uid="{1B439FAA-0761-C44E-965D-469A22852A8F}" name="Transaction Date" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{1B439FAA-0761-C44E-965D-469A22852A8F}" name="Transaction Date" dataDxfId="41"/>
     <tableColumn id="3" xr3:uid="{CC2B1945-8262-9145-9F19-C2DE98427053}" name="Category"/>
     <tableColumn id="4" xr3:uid="{A13631DC-44F7-D247-9F04-999BA9E49159}" name="Merchant"/>
     <tableColumn id="5" xr3:uid="{92221C3F-3723-3E46-9028-2994DF171F8A}" name="Amount ($)"/>
-    <tableColumn id="9" xr3:uid="{5E07B6B1-B6A7-FD45-A36B-AE02CF6A75AA}" name="Spending or Income" dataDxfId="37">
+    <tableColumn id="9" xr3:uid="{5E07B6B1-B6A7-FD45-A36B-AE02CF6A75AA}" name="Spending or Income" dataDxfId="40">
       <calculatedColumnFormula>IF(expenses_table[[#This Row],[Amount ($)]]&lt;0, "Spending", "Income")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{C747EDCA-AF62-A541-9179-3179FBEC7C11}" name="Need/Want"/>
-    <tableColumn id="7" xr3:uid="{38B9BC3B-CEB7-1246-A416-997FA882D8A9}" name="Month" dataDxfId="36">
+    <tableColumn id="7" xr3:uid="{38B9BC3B-CEB7-1246-A416-997FA882D8A9}" name="Month" dataDxfId="39">
       <calculatedColumnFormula>TEXT(expenses_table[[#This Row],[Transaction Date]], "mmmm")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{821F97FE-09B4-E647-907B-FEFE3B9E94F7}" name="Workday/Extended Weekend (inc Friday)" dataDxfId="35">
+    <tableColumn id="8" xr3:uid="{821F97FE-09B4-E647-907B-FEFE3B9E94F7}" name="Workday/Extended Weekend (inc Friday)" dataDxfId="38">
       <calculatedColumnFormula>IF(WEEKDAY(expenses_table[[#This Row],[Transaction Date]], 2) &lt;= 4, "Workday", "Ext-Weekend")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13542,7 +13637,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1B6A8F48-A898-7B41-8B2F-2C8E9106DD5A}" name="earnings_table" displayName="earnings_table" ref="A1:I247" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1B6A8F48-A898-7B41-8B2F-2C8E9106DD5A}" name="earnings_table" displayName="earnings_table" ref="A1:I247" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="A1:I247" xr:uid="{1B6A8F48-A898-7B41-8B2F-2C8E9106DD5A}">
     <filterColumn colId="2">
       <filters>
@@ -13558,22 +13653,22 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{31B2C3DA-4854-9844-9496-96146F16A89E}" name="Method" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{F71D2D76-F449-6846-A86A-31D132D01864}" name="Transaction Date" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{698BE150-94AA-6647-A4A5-F0D1632492E8}" name="Category" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{62EA866A-6213-BE46-A5CC-E8DAC9C406A8}" name="Merchant" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{28935B6D-449E-5A45-AA26-1E8220AE2B4F}" name="Amount ($)" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{FD1C89E1-120E-994B-B144-AC49F06A5BCE}" name="Spending or Income" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{5DA1230D-54BC-734B-A7E7-501E0542A11B}" name="Need/Want" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{B107A14D-0255-0149-B572-B678995ADF37}" name="Month" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{B38D5AA0-A0B8-E54B-84D7-E0C0E1511AE4}" name="Workday/Extended Weekend (inc Friday)" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{31B2C3DA-4854-9844-9496-96146F16A89E}" name="Method" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{F71D2D76-F449-6846-A86A-31D132D01864}" name="Transaction Date" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{698BE150-94AA-6647-A4A5-F0D1632492E8}" name="Category" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{62EA866A-6213-BE46-A5CC-E8DAC9C406A8}" name="Merchant" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{28935B6D-449E-5A45-AA26-1E8220AE2B4F}" name="Amount ($)" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{FD1C89E1-120E-994B-B144-AC49F06A5BCE}" name="Spending or Income" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{5DA1230D-54BC-734B-A7E7-501E0542A11B}" name="Need/Want" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{B107A14D-0255-0149-B572-B678995ADF37}" name="Month" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{B38D5AA0-A0B8-E54B-84D7-E0C0E1511AE4}" name="Workday/Extended Weekend (inc Friday)" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E0EF351-E274-B742-BA70-BF66AF535AA2}" name="clean_table" displayName="clean_table" ref="A1:I247" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E0EF351-E274-B742-BA70-BF66AF535AA2}" name="clean_table" displayName="clean_table" ref="A1:I247" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11">
   <autoFilter ref="A1:I247" xr:uid="{2E0EF351-E274-B742-BA70-BF66AF535AA2}">
     <filterColumn colId="2">
       <filters>
@@ -13599,18 +13694,18 @@
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A3AC953F-C3BF-EC4D-BED6-3CD2101D70CB}" name="Method"/>
-    <tableColumn id="2" xr3:uid="{A5BF0BD9-2C81-0044-A20C-49D5AAB02C7F}" name="Transaction Date" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{A5BF0BD9-2C81-0044-A20C-49D5AAB02C7F}" name="Transaction Date" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{1F839404-3984-5942-A4B6-A0BA5517ECBE}" name="Category"/>
     <tableColumn id="4" xr3:uid="{2E492010-3649-CE4D-B40E-51953B8AA2B4}" name="Merchant"/>
     <tableColumn id="5" xr3:uid="{DA92C096-E88D-5247-9AFF-65920543CDCF}" name="Amount ($)"/>
-    <tableColumn id="9" xr3:uid="{7C9899EE-AB63-5148-93CF-F8AFDDB6142C}" name="Spending or Income" dataDxfId="5">
+    <tableColumn id="9" xr3:uid="{7C9899EE-AB63-5148-93CF-F8AFDDB6142C}" name="Spending or Income" dataDxfId="9">
       <calculatedColumnFormula>IF(clean_table[[#This Row],[Amount ($)]]&lt;0, "Spending", "Income")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{F75F65BF-D5DF-BB45-A978-62BAC39848E0}" name="Need/Want"/>
-    <tableColumn id="7" xr3:uid="{AD3A5953-37D8-9346-8570-AF420D890048}" name="Month" dataDxfId="4">
+    <tableColumn id="7" xr3:uid="{AD3A5953-37D8-9346-8570-AF420D890048}" name="Month" dataDxfId="8">
       <calculatedColumnFormula>TEXT(clean_table[[#This Row],[Transaction Date]], "mmmm")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2C48890E-6BA1-834F-8B9C-C6D4CD51ADFD}" name="Workday/Extended Weekend (inc Friday)" dataDxfId="3">
+    <tableColumn id="8" xr3:uid="{2C48890E-6BA1-834F-8B9C-C6D4CD51ADFD}" name="Workday/Extended Weekend (inc Friday)" dataDxfId="7">
       <calculatedColumnFormula>IF(WEEKDAY(clean_table[[#This Row],[Transaction Date]], 2) &lt;= 4, "Workday", "Ext-Weekend")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13907,79 +14002,79 @@
   <sheetData>
     <row r="2" spans="2:12" ht="4" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:12" ht="35" x14ac:dyDescent="0.35">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+    </row>
+    <row r="5" spans="2:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+    </row>
+    <row r="6" spans="2:12" ht="23" x14ac:dyDescent="0.25">
+      <c r="B6" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+    </row>
+    <row r="9" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="B9" s="47" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="B11" s="40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="B12" s="41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="B15" s="47" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="190" x14ac:dyDescent="0.2">
+      <c r="B16" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-    </row>
-    <row r="5" spans="2:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-    </row>
-    <row r="6" spans="2:12" ht="23" x14ac:dyDescent="0.25">
-      <c r="B6" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-    </row>
-    <row r="9" spans="2:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="B9" s="52" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="B11" s="41" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="B12" s="42" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="B15" s="52" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" ht="190" x14ac:dyDescent="0.2">
-      <c r="B16" s="54" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="19" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="47" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B20" s="41" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="B20" s="42" t="s">
-        <v>114</v>
-      </c>
-    </row>
     <row r="23" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="42" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="23" x14ac:dyDescent="0.25">
       <c r="A24" s="39"/>
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="50" t="s">
         <v>98</v>
       </c>
     </row>
@@ -13991,20 +14086,20 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7FE9DA-4A4C-C24B-A585-638A6FA80252}">
-  <dimension ref="A2:K19"/>
+  <dimension ref="B4:K20"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="137" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="131" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.83203125" customWidth="1"/>
     <col min="7" max="7" width="6.6640625" customWidth="1"/>
     <col min="8" max="8" width="7.6640625" customWidth="1"/>
     <col min="9" max="9" width="5.6640625" customWidth="1"/>
@@ -14020,257 +14115,255 @@
     <col min="19" max="19" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="50" t="s">
+    <row r="4" spans="2:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B4" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="C4" s="57" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="40" t="s">
+    <row r="5" spans="2:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B5" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="57" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A5" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="F5" s="48" t="s">
+      <c r="G5" s="46" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="50" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="46"/>
-      <c r="I6" s="2"/>
+    <row r="6" spans="2:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="G6" s="44"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49">
-        <v>-140</v>
-      </c>
-      <c r="D7" s="49">
-        <v>-140</v>
-      </c>
-      <c r="F7" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="I7" s="3"/>
+    <row r="7" spans="2:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="B7" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="G7" s="45" t="s">
+        <v>110</v>
+      </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="49">
-        <v>-772.44999999999993</v>
-      </c>
-      <c r="C8" s="49">
-        <v>-292.57</v>
-      </c>
-      <c r="D8" s="49">
-        <v>-1065.02</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="I8" s="2"/>
+    <row r="8" spans="2:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="B8" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="45" t="s">
+        <v>109</v>
+      </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49">
-        <v>-9.24</v>
-      </c>
-      <c r="D9" s="49">
-        <v>-9.24</v>
+    <row r="9" spans="2:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B9" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60">
+        <v>-140</v>
+      </c>
+      <c r="E9" s="60">
+        <v>-140</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="49">
-        <v>-195.11</v>
-      </c>
-      <c r="C10" s="49">
-        <v>-45</v>
-      </c>
-      <c r="D10" s="49">
-        <v>-240.11</v>
+    <row r="10" spans="2:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B10" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="60">
+        <v>-772.44999999999993</v>
+      </c>
+      <c r="D10" s="60">
+        <v>-292.57</v>
+      </c>
+      <c r="E10" s="60">
+        <v>-1065.02</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="51" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="49">
-        <v>-2.99</v>
-      </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49">
-        <v>-2.99</v>
+    <row r="11" spans="2:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B11" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60">
+        <v>-9.24</v>
+      </c>
+      <c r="E11" s="60">
+        <v>-9.24</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="49">
-        <v>-33.9</v>
-      </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49">
-        <v>-33.9</v>
+    <row r="12" spans="2:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B12" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="60">
+        <v>-195.11</v>
+      </c>
+      <c r="D12" s="60">
+        <v>-45</v>
+      </c>
+      <c r="E12" s="60">
+        <v>-240.11</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="51" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="49">
-        <v>-161.44</v>
-      </c>
-      <c r="C13" s="49">
-        <v>-312.88999999999987</v>
-      </c>
-      <c r="D13" s="49">
-        <v>-474.32999999999987</v>
+    <row r="13" spans="2:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B13" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="60">
+        <v>-2.99</v>
+      </c>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60">
+        <v>-2.99</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49">
-        <v>-42.26</v>
-      </c>
-      <c r="D14" s="49">
-        <v>-42.26</v>
+    <row r="14" spans="2:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B14" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="60">
+        <v>-33.9</v>
+      </c>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60">
+        <v>-33.9</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="49">
-        <v>-538.66999999999996</v>
-      </c>
-      <c r="C15" s="49">
-        <v>-390.43000000000006</v>
-      </c>
-      <c r="D15" s="49">
-        <v>-929.1</v>
+    <row r="15" spans="2:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B15" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="60">
+        <v>-161.44</v>
+      </c>
+      <c r="D15" s="60">
+        <v>-312.88999999999987</v>
+      </c>
+      <c r="E15" s="60">
+        <v>-474.32999999999987</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="49">
-        <v>-112</v>
-      </c>
-      <c r="C16" s="49">
-        <v>-639.5</v>
-      </c>
-      <c r="D16" s="49">
-        <v>-751.5</v>
+    <row r="16" spans="2:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B16" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60">
+        <v>-42.26</v>
+      </c>
+      <c r="E16" s="60">
+        <v>-42.26</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="49">
-        <v>-146.88999999999999</v>
-      </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49">
-        <v>-146.88999999999999</v>
+    <row r="17" spans="2:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B17" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="60">
+        <v>-538.66999999999996</v>
+      </c>
+      <c r="D17" s="60">
+        <v>-390.43000000000006</v>
+      </c>
+      <c r="E17" s="60">
+        <v>-929.1</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="49">
-        <v>-1963.4499999999998</v>
-      </c>
-      <c r="C18" s="49">
-        <v>-1871.8899999999999</v>
-      </c>
-      <c r="D18" s="49">
-        <v>-3835.3399999999997</v>
+    <row r="18" spans="2:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B18" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="60">
+        <v>-112</v>
+      </c>
+      <c r="D18" s="60">
+        <v>-639.5</v>
+      </c>
+      <c r="E18" s="60">
+        <v>-751.5</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B19" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="60">
+        <v>-146.88999999999999</v>
+      </c>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60">
+        <v>-146.88999999999999</v>
+      </c>
       <c r="I19" s="4"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
+    <row r="20" spans="2:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B20" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="59">
+        <v>-1963.4499999999998</v>
+      </c>
+      <c r="D20" s="59">
+        <v>-1871.8899999999999</v>
+      </c>
+      <c r="E20" s="59">
+        <v>-3835.3399999999997</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId2"/>
@@ -22217,7 +22310,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B813E8-23BF-FF44-B015-1FE81D517B4E}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="172" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
@@ -22246,153 +22339,145 @@
       </c>
       <c r="D3" t="str" cm="1">
         <f t="array" ref="D3:D12">A4:A13</f>
-        <v>Transportation</v>
+        <v>Entertainment</v>
       </c>
       <c r="E3" cm="1">
         <f t="array" ref="E3:E12">ABS(B4:B13)</f>
-        <v>1065.02</v>
+        <v>929.1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="61">
-        <v>-1065.02</v>
+        <v>15</v>
+      </c>
+      <c r="B4" s="62">
+        <v>-929.1</v>
       </c>
       <c r="D4" t="str">
-        <v>Entertainment</v>
+        <v>E-Transfer</v>
       </c>
       <c r="E4">
-        <v>929.1</v>
+        <v>751.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="61">
-        <v>-929.1</v>
+        <v>6</v>
+      </c>
+      <c r="B5" s="62">
+        <v>-751.5</v>
       </c>
       <c r="D5" t="str">
-        <v>E-Transfer</v>
+        <v>Food</v>
       </c>
       <c r="E5">
-        <v>751.5</v>
+        <v>474.33000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="61">
-        <v>-751.5</v>
+        <v>12</v>
+      </c>
+      <c r="B6" s="62">
+        <v>-474.33000000000004</v>
       </c>
       <c r="D6" t="str">
-        <v>Food</v>
+        <v>Healthcare</v>
       </c>
       <c r="E6">
-        <v>474.3300000000001</v>
+        <v>240.11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="61">
-        <v>-474.3300000000001</v>
+        <v>25</v>
+      </c>
+      <c r="B7" s="62">
+        <v>-240.11</v>
       </c>
       <c r="D7" t="str">
-        <v>Healthcare</v>
+        <v>Clothing</v>
       </c>
       <c r="E7">
-        <v>240.11</v>
+        <v>146.88999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="61">
-        <v>-240.11</v>
+        <v>62</v>
+      </c>
+      <c r="B8" s="62">
+        <v>-146.88999999999999</v>
       </c>
       <c r="D8" t="str">
-        <v>Clothing</v>
+        <v>Fitness</v>
       </c>
       <c r="E8">
-        <v>146.88999999999999</v>
+        <v>42.26</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="61">
-        <v>-146.88999999999999</v>
+        <v>44</v>
+      </c>
+      <c r="B9" s="62">
+        <v>-42.26</v>
       </c>
       <c r="D9" t="str">
-        <v>Fitness</v>
+        <v>Gift</v>
       </c>
       <c r="E9">
-        <v>42.26</v>
+        <v>33.9</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="61">
-        <v>-42.26</v>
+        <v>20</v>
+      </c>
+      <c r="B10" s="62">
+        <v>-33.9</v>
       </c>
       <c r="D10" t="str">
-        <v>Gift</v>
+        <v>Other</v>
       </c>
       <c r="E10">
-        <v>33.9</v>
+        <v>9.24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="61">
-        <v>-33.9</v>
+        <v>30</v>
+      </c>
+      <c r="B11" s="62">
+        <v>-9.24</v>
       </c>
       <c r="D11" t="str">
-        <v>Other</v>
+        <v>Grocery</v>
       </c>
       <c r="E11">
-        <v>9.24</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="61">
-        <v>-9.24</v>
+        <v>37</v>
+      </c>
+      <c r="B12" s="62">
+        <v>-2.99</v>
       </c>
       <c r="D12" t="str">
-        <v>Grocery</v>
+        <v>Grand Total</v>
       </c>
       <c r="E12">
-        <v>2.99</v>
+        <v>2630.3199999999997</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="61">
-        <v>-2.99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="61">
-        <v>-3695.3399999999997</v>
+      <c r="B13" s="62">
+        <v>-2630.3199999999997</v>
       </c>
     </row>
   </sheetData>
@@ -22408,7 +22493,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4B15A5-4555-0B44-BDCF-73A7E44CEA5F}">
-  <dimension ref="A3:B45"/>
+  <dimension ref="A3:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -22430,338 +22515,298 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="61">
-        <v>-575</v>
+        <v>59</v>
+      </c>
+      <c r="B4" s="62">
+        <v>-170</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="61">
-        <v>-231.44</v>
+        <v>66</v>
+      </c>
+      <c r="B5" s="62">
+        <v>-128.13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="61">
-        <v>-208.32999999999998</v>
+        <v>14</v>
+      </c>
+      <c r="B6" s="62">
+        <v>-111.64999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="61">
-        <v>-170</v>
+        <v>63</v>
+      </c>
+      <c r="B7" s="62">
+        <v>-101.69</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="61">
-        <v>-128.13</v>
+        <v>49</v>
+      </c>
+      <c r="B8" s="62">
+        <v>-86.37</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="61">
-        <v>-111.64999999999998</v>
+        <v>23</v>
+      </c>
+      <c r="B9" s="62">
+        <v>-84.22999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="61">
-        <v>-101.69</v>
+        <v>70</v>
+      </c>
+      <c r="B10" s="62">
+        <v>-73.36</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="61">
-        <v>-86.37</v>
+        <v>54</v>
+      </c>
+      <c r="B11" s="62">
+        <v>-67.48</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="61">
-        <v>-84.22999999999999</v>
+        <v>71</v>
+      </c>
+      <c r="B12" s="62">
+        <v>-56.65</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="61">
-        <v>-73.36</v>
+        <v>45</v>
+      </c>
+      <c r="B13" s="62">
+        <v>-53.56</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="61">
-        <v>-67.48</v>
+        <v>39</v>
+      </c>
+      <c r="B14" s="62">
+        <v>-53.34</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="61">
-        <v>-56.65</v>
+        <v>69</v>
+      </c>
+      <c r="B15" s="62">
+        <v>-51.02</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="61">
-        <v>-53.56</v>
+        <v>68</v>
+      </c>
+      <c r="B16" s="62">
+        <v>-49.72</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="61">
-        <v>-53.34</v>
+        <v>58</v>
+      </c>
+      <c r="B17" s="62">
+        <v>-48.300000000000004</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="61">
-        <v>-51.02</v>
+        <v>41</v>
+      </c>
+      <c r="B18" s="62">
+        <v>-46.43</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="61">
-        <v>-49.72</v>
+        <v>64</v>
+      </c>
+      <c r="B19" s="62">
+        <v>-45.2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="61">
-        <v>-48.300000000000004</v>
+        <v>26</v>
+      </c>
+      <c r="B20" s="62">
+        <v>-36.21</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="61">
-        <v>-46.43</v>
+        <v>61</v>
+      </c>
+      <c r="B21" s="62">
+        <v>-33.9</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="61">
-        <v>-45.2</v>
+        <v>21</v>
+      </c>
+      <c r="B22" s="62">
+        <v>-33.9</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="61">
-        <v>-36.21</v>
+        <v>65</v>
+      </c>
+      <c r="B23" s="62">
+        <v>-33.880000000000003</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="61">
-        <v>-34.450000000000003</v>
+        <v>28</v>
+      </c>
+      <c r="B24" s="62">
+        <v>-31.830000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="61">
-        <v>-33.9</v>
+        <v>36</v>
+      </c>
+      <c r="B25" s="62">
+        <v>-24.26</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="61">
-        <v>-33.9</v>
+        <v>51</v>
+      </c>
+      <c r="B26" s="62">
+        <v>-22.6</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B27" s="61">
-        <v>-33.880000000000003</v>
+        <v>53</v>
+      </c>
+      <c r="B27" s="62">
+        <v>-21.840000000000003</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="61">
-        <v>-31.830000000000002</v>
+        <v>46</v>
+      </c>
+      <c r="B28" s="62">
+        <v>-20.11</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="61">
-        <v>-24.26</v>
+        <v>67</v>
+      </c>
+      <c r="B29" s="62">
+        <v>-16.940000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="61">
-        <v>-22.6</v>
+        <v>50</v>
+      </c>
+      <c r="B30" s="62">
+        <v>-16.100000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="61">
-        <v>-21.840000000000003</v>
+        <v>19</v>
+      </c>
+      <c r="B31" s="62">
+        <v>-15.18</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="61">
-        <v>-20.11</v>
+        <v>35</v>
+      </c>
+      <c r="B32" s="62">
+        <v>-14.38</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="61">
-        <v>-16.940000000000001</v>
+        <v>22</v>
+      </c>
+      <c r="B33" s="62">
+        <v>-14.16</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="61">
-        <v>-16.100000000000001</v>
+        <v>40</v>
+      </c>
+      <c r="B34" s="62">
+        <v>-10.46</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="61">
-        <v>-15.8</v>
+        <v>55</v>
+      </c>
+      <c r="B35" s="62">
+        <v>-10.17</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="61">
-        <v>-15.18</v>
+        <v>29</v>
+      </c>
+      <c r="B36" s="62">
+        <v>-4.5999999999999996</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="61">
-        <v>-14.38</v>
+        <v>13</v>
+      </c>
+      <c r="B37" s="62">
+        <v>-4.08</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="61">
-        <v>-14.16</v>
+        <v>38</v>
+      </c>
+      <c r="B38" s="62">
+        <v>-2.99</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="61">
-        <v>-10.46</v>
+        <v>9</v>
+      </c>
+      <c r="B39" s="62">
+        <v>4930.82</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B40" s="61">
-        <v>-10.17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41" s="61">
-        <v>-4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" s="61">
-        <v>-4.08</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43" s="61">
-        <v>-2.99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" s="61">
-        <v>4930.8200000000006</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="61">
-        <v>2271.0800000000004</v>
+      <c r="B40" s="62">
+        <v>3336.1000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -37954,7 +37999,7 @@
         <v>74</v>
       </c>
       <c r="B6" s="9">
-        <v>-1032.8100000000002</v>
+        <v>-765.30000000000018</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -37965,7 +38010,7 @@
         <v>75</v>
       </c>
       <c r="B7" s="9">
-        <v>-680.70999999999992</v>
+        <v>-535.68000000000006</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="2"/>
@@ -37976,7 +38021,7 @@
         <v>76</v>
       </c>
       <c r="B8" s="9">
-        <v>-1253.9899999999996</v>
+        <v>-841.40000000000009</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -37987,7 +38032,7 @@
         <v>77</v>
       </c>
       <c r="B9" s="9">
-        <v>-727.83</v>
+        <v>-487.93999999999994</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="2"/>
@@ -37998,7 +38043,7 @@
         <v>78</v>
       </c>
       <c r="B10" s="9">
-        <v>-3695.3399999999992</v>
+        <v>-2630.32</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="2"/>
@@ -38140,8 +38185,8 @@
   </sheetPr>
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38157,24 +38202,24 @@
   <sheetData>
     <row r="1" spans="1:17" ht="59" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5"/>
-      <c r="B1" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
+      <c r="B1" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
@@ -38188,8 +38233,8 @@
     </row>
     <row r="6" spans="1:17" ht="45" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
-      <c r="B6" s="45" t="s">
-        <v>100</v>
+      <c r="B6" s="63" t="s">
+        <v>114</v>
       </c>
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
@@ -38223,7 +38268,7 @@
       </c>
       <c r="I11" s="27">
         <f>GETPIVOTDATA("Amount ($)",PivotExpenses_Chart!$A$5)</f>
-        <v>-3695.3399999999992</v>
+        <v>-2630.32</v>
       </c>
       <c r="J11" s="25"/>
     </row>
@@ -38245,7 +38290,7 @@
       </c>
       <c r="I13" s="29">
         <f>I12+I11</f>
-        <v>2259.09</v>
+        <v>3324.1099999999992</v>
       </c>
       <c r="J13" s="25"/>
     </row>
@@ -38267,29 +38312,29 @@
     <row r="17" spans="1:10" ht="23" x14ac:dyDescent="0.25">
       <c r="H17" s="36" t="str" cm="1">
         <f t="array" ref="H17:I19">PivotCategory_Chart!A4:B6</f>
-        <v>Transportation</v>
+        <v>Entertainment</v>
       </c>
       <c r="I17" s="30">
-        <v>-1065.02</v>
+        <v>-929.1</v>
       </c>
       <c r="J17" s="25"/>
     </row>
     <row r="18" spans="1:10" ht="23" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="H18" s="37" t="str">
-        <v>Entertainment</v>
+        <v>E-Transfer</v>
       </c>
       <c r="I18" s="28">
-        <v>-929.1</v>
+        <v>-751.5</v>
       </c>
       <c r="J18" s="25"/>
     </row>
     <row r="19" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H19" s="35" t="str">
-        <v>E-Transfer</v>
+        <v>Food</v>
       </c>
       <c r="I19" s="29">
-        <v>-751.5</v>
+        <v>-474.33000000000004</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -38312,27 +38357,27 @@
       <c r="A23" s="3"/>
       <c r="H23" s="36" t="str" cm="1">
         <f t="array" ref="H23:I25">PivotMerchant_Calculation!A4:B6</f>
-        <v>Uber</v>
+        <v>Trinibago Haircuts</v>
       </c>
       <c r="I23" s="30">
-        <v>-575</v>
+        <v>-170</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="23" x14ac:dyDescent="0.25">
       <c r="H24" s="37" t="str">
-        <v>Esso Circle</v>
+        <v>Petty Cash</v>
       </c>
       <c r="I24" s="28">
-        <v>-231.44</v>
+        <v>-128.13</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="H25" s="35" t="str">
-        <v>Costco</v>
+        <v>Gino's Pizza</v>
       </c>
       <c r="I25" s="29">
-        <v>-208.32999999999998</v>
+        <v>-111.64999999999998</v>
       </c>
     </row>
     <row r="33" spans="9:10" ht="18" x14ac:dyDescent="0.2">
@@ -38340,7 +38385,7 @@
       <c r="J33" s="26"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" pivotTables="0"/>
   <mergeCells count="1">
     <mergeCell ref="B1:Q1"/>
   </mergeCells>
@@ -38366,9 +38411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81B38CC-D398-E648-A50E-2BDC2C61B0BE}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="151" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
-    </sheetView>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="151" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -38381,210 +38424,210 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="57" t="s">
+      <c r="A2" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="52" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59">
+      <c r="B6" s="54"/>
+      <c r="C6" s="54">
         <v>1132.95</v>
       </c>
-      <c r="D6" s="59">
+      <c r="D6" s="54">
         <v>44</v>
       </c>
-      <c r="E6" s="59">
+      <c r="E6" s="54">
         <v>1176.95</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59">
+      <c r="B7" s="54"/>
+      <c r="C7" s="54">
         <v>1040.3900000000001</v>
       </c>
-      <c r="D7" s="59">
+      <c r="D7" s="54">
         <v>332</v>
       </c>
-      <c r="E7" s="59">
+      <c r="E7" s="54">
         <v>1372.39</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="59">
+      <c r="B8" s="54">
         <v>225</v>
       </c>
-      <c r="C8" s="59">
+      <c r="C8" s="54">
         <v>2037.5</v>
       </c>
-      <c r="D8" s="59">
+      <c r="D8" s="54">
         <v>765.72</v>
       </c>
-      <c r="E8" s="59">
+      <c r="E8" s="54">
         <v>3028.2200000000003</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59">
+      <c r="B9" s="54"/>
+      <c r="C9" s="54">
         <v>723.73</v>
       </c>
-      <c r="D9" s="59">
+      <c r="D9" s="54">
         <v>328.14</v>
       </c>
-      <c r="E9" s="59">
+      <c r="E9" s="54">
         <v>1051.8699999999999</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="59">
+      <c r="B10" s="54">
         <v>225</v>
       </c>
-      <c r="C10" s="59">
+      <c r="C10" s="54">
         <v>4934.57</v>
       </c>
-      <c r="D10" s="59">
+      <c r="D10" s="54">
         <v>1469.8600000000001</v>
       </c>
-      <c r="E10" s="59">
+      <c r="E10" s="54">
         <v>6629.43</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="57"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="57"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="57"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
+      <c r="A13" s="52"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="57"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
+      <c r="A14" s="52"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="57"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="57"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="57"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
     </row>
     <row r="20" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="G20" s="48" t="s">
+      <c r="G20" s="46" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="G21" s="46"/>
+      <c r="G21" s="44"/>
     </row>
     <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="G22" s="47" t="s">
+      <c r="G22" s="45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="G23" s="45" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="G23" s="47" t="s">
-        <v>109</v>
-      </c>
-    </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
   <extLst>

</xml_diff>